<commit_message>
Update for the Documents 23.01.18
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/Gruppen-Planung.xlsx
+++ b/01_ProjectPlanning/Gruppen-Planung.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="84">
   <si>
     <t>Task</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>Drawing new Background for second Level</t>
+  </si>
+  <si>
+    <t>Drawing Clouds for the second Level</t>
+  </si>
+  <si>
+    <t>Implementing scrolling of the Clouds</t>
   </si>
 </sst>
 </file>
@@ -816,7 +822,7 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2737,19 +2743,21 @@
         <v>2</v>
       </c>
       <c r="C57" s="1">
+        <v>3</v>
+      </c>
+      <c r="D57" s="1">
         <v>2</v>
       </c>
-      <c r="D57" s="1"/>
       <c r="E57" s="1">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G57" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>0.66666666666666674</v>
       </c>
       <c r="H57" s="12" t="str">
         <f t="shared" si="12"/>
@@ -2771,21 +2779,23 @@
       <c r="C58" s="1">
         <v>2</v>
       </c>
-      <c r="D58" s="1"/>
+      <c r="D58" s="1">
+        <v>2</v>
+      </c>
       <c r="E58" s="1">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G58" s="3">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>X</v>
+        <v>✔</v>
       </c>
       <c r="I58" s="12">
         <v>10</v>
@@ -2794,46 +2804,70 @@
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+      <c r="A59" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2</v>
+      </c>
       <c r="E59" s="1">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F59" s="1"/>
-      <c r="G59" s="3" t="e">
+      <c r="F59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G59" s="3">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H59" s="12" t="e">
+        <v>1</v>
+      </c>
+      <c r="H59" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I59" s="12"/>
+        <v>✔</v>
+      </c>
+      <c r="I59" s="12">
+        <v>10</v>
+      </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+      <c r="A60" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="1">
+        <v>3</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1">
+        <v>3</v>
+      </c>
       <c r="E60" s="1">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="3" t="e">
+      <c r="F60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="3">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H60" s="12" t="e">
+        <v>1</v>
+      </c>
+      <c r="H60" s="12" t="str">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I60" s="12"/>
+        <v>✔</v>
+      </c>
+      <c r="I60" s="12">
+        <v>10</v>
+      </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>

</xml_diff>